<commit_message>
Docs + Limpeza c?digo
</commit_message>
<xml_diff>
--- a/docs/Log_Gestao_Projecto_aluno1_1100554.xlsx
+++ b/docs/Log_Gestao_Projecto_aluno1_1100554.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Lista de Itens" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -1854,6 +1854,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1932,9 +1935,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1950,7 +1950,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2382,20 +2382,20 @@
       <c r="C22" s="19"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="52"/>
+      <c r="C23" s="53"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
     </row>
     <row r="25" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="54"/>
+      <c r="C25" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2423,58 +2423,58 @@
   <sheetData>
     <row r="1" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="58"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="60"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="61"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="60"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="61"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="63"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="64"/>
     </row>
     <row r="6" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -2486,10 +2486,10 @@
       <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="8">
         <v>41078</v>
       </c>
@@ -2767,50 +2767,50 @@
   <sheetData>
     <row r="1" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="60"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -3281,10 +3281,10 @@
   <dimension ref="A1:I281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="C132" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="11" topLeftCell="C113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="F137" sqref="F137"/>
+      <selection pane="bottomRight" activeCell="I111" sqref="I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3296,61 +3296,61 @@
   <sheetData>
     <row r="1" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="60"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="60"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="61"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="63"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -4965,74 +4965,74 @@
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="65" t="s">
+      <c r="A98" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B98" s="66"/>
-      <c r="C98" s="66"/>
-      <c r="D98" s="66"/>
-      <c r="E98" s="66"/>
-      <c r="F98" s="66"/>
-      <c r="G98" s="66"/>
-      <c r="H98" s="66"/>
-      <c r="I98" s="67"/>
+      <c r="B98" s="67"/>
+      <c r="C98" s="67"/>
+      <c r="D98" s="67"/>
+      <c r="E98" s="67"/>
+      <c r="F98" s="67"/>
+      <c r="G98" s="67"/>
+      <c r="H98" s="67"/>
+      <c r="I98" s="68"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="68" t="s">
+      <c r="A99" s="69" t="s">
         <v>247</v>
       </c>
-      <c r="B99" s="69"/>
-      <c r="C99" s="69"/>
-      <c r="D99" s="69"/>
-      <c r="E99" s="69"/>
-      <c r="F99" s="69"/>
-      <c r="G99" s="69"/>
-      <c r="H99" s="69"/>
-      <c r="I99" s="70"/>
+      <c r="B99" s="70"/>
+      <c r="C99" s="70"/>
+      <c r="D99" s="70"/>
+      <c r="E99" s="70"/>
+      <c r="F99" s="70"/>
+      <c r="G99" s="70"/>
+      <c r="H99" s="70"/>
+      <c r="I99" s="71"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="71"/>
-      <c r="B100" s="72"/>
-      <c r="C100" s="72"/>
-      <c r="D100" s="72"/>
-      <c r="E100" s="72"/>
-      <c r="F100" s="72"/>
-      <c r="G100" s="72"/>
-      <c r="H100" s="72"/>
-      <c r="I100" s="73"/>
+      <c r="A100" s="72"/>
+      <c r="B100" s="73"/>
+      <c r="C100" s="73"/>
+      <c r="D100" s="73"/>
+      <c r="E100" s="73"/>
+      <c r="F100" s="73"/>
+      <c r="G100" s="73"/>
+      <c r="H100" s="73"/>
+      <c r="I100" s="74"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="71"/>
-      <c r="B101" s="72"/>
-      <c r="C101" s="72"/>
-      <c r="D101" s="72"/>
-      <c r="E101" s="72"/>
-      <c r="F101" s="72"/>
-      <c r="G101" s="72"/>
-      <c r="H101" s="72"/>
-      <c r="I101" s="73"/>
+      <c r="A101" s="72"/>
+      <c r="B101" s="73"/>
+      <c r="C101" s="73"/>
+      <c r="D101" s="73"/>
+      <c r="E101" s="73"/>
+      <c r="F101" s="73"/>
+      <c r="G101" s="73"/>
+      <c r="H101" s="73"/>
+      <c r="I101" s="74"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="71"/>
-      <c r="B102" s="72"/>
-      <c r="C102" s="72"/>
-      <c r="D102" s="72"/>
-      <c r="E102" s="72"/>
-      <c r="F102" s="72"/>
-      <c r="G102" s="72"/>
-      <c r="H102" s="72"/>
-      <c r="I102" s="73"/>
+      <c r="A102" s="72"/>
+      <c r="B102" s="73"/>
+      <c r="C102" s="73"/>
+      <c r="D102" s="73"/>
+      <c r="E102" s="73"/>
+      <c r="F102" s="73"/>
+      <c r="G102" s="73"/>
+      <c r="H102" s="73"/>
+      <c r="I102" s="74"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="74"/>
-      <c r="B103" s="75"/>
-      <c r="C103" s="75"/>
-      <c r="D103" s="75"/>
-      <c r="E103" s="75"/>
-      <c r="F103" s="75"/>
-      <c r="G103" s="75"/>
-      <c r="H103" s="75"/>
-      <c r="I103" s="76"/>
+      <c r="A103" s="75"/>
+      <c r="B103" s="76"/>
+      <c r="C103" s="76"/>
+      <c r="D103" s="76"/>
+      <c r="E103" s="76"/>
+      <c r="F103" s="76"/>
+      <c r="G103" s="76"/>
+      <c r="H103" s="76"/>
+      <c r="I103" s="77"/>
     </row>
     <row r="105" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
@@ -5080,7 +5080,7 @@
       <c r="A109" t="s">
         <v>179</v>
       </c>
-      <c r="B109" s="77" t="s">
+      <c r="B109" s="51" t="s">
         <v>180</v>
       </c>
       <c r="C109">
@@ -5112,7 +5112,7 @@
       <c r="G110" s="35"/>
       <c r="H110" s="35"/>
       <c r="I110" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -5133,7 +5133,7 @@
       <c r="G111" s="35"/>
       <c r="H111" s="35"/>
       <c r="I111" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -5154,7 +5154,7 @@
       <c r="G112" s="35"/>
       <c r="H112" s="35"/>
       <c r="I112" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
@@ -5175,7 +5175,7 @@
       <c r="G113" s="35"/>
       <c r="H113" s="35"/>
       <c r="I113" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
       <c r="G114" s="35"/>
       <c r="H114" s="35"/>
       <c r="I114" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -5217,7 +5217,7 @@
       <c r="G115" s="35"/>
       <c r="H115" s="35"/>
       <c r="I115" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -5238,7 +5238,7 @@
       <c r="G116" s="35"/>
       <c r="H116" s="35"/>
       <c r="I116" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -5259,7 +5259,7 @@
       <c r="G117" s="35"/>
       <c r="H117" s="35"/>
       <c r="I117" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
       <c r="G118" s="35"/>
       <c r="H118" s="35"/>
       <c r="I118" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -5301,7 +5301,7 @@
       <c r="G119" s="35"/>
       <c r="H119" s="35"/>
       <c r="I119" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Relotorio Tecnico, Log Individual, GP
</commit_message>
<xml_diff>
--- a/docs/Log_Gestao_Projecto_aluno1_1100554.xlsx
+++ b/docs/Log_Gestao_Projecto_aluno1_1100554.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="11640" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="7935" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Lista de Itens" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -699,7 +699,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="249">
   <si>
     <t>Plano de Sprint</t>
   </si>
@@ -1488,6 +1488,9 @@
   </si>
   <si>
     <t>Algumas áreas ficaram sem testes unitários, embora estivessem planeados. A iteração 1 foi concluída com sucesso, tendo ficado todos os requisitos funcionais.</t>
+  </si>
+  <si>
+    <t>Desenvolvimento codigo importação</t>
   </si>
 </sst>
 </file>
@@ -1950,7 +1953,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2748,10 +2751,10 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3281,10 +3284,10 @@
   <dimension ref="A1:I281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="C113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="11" topLeftCell="C134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="I111" sqref="I111"/>
+      <selection pane="bottomRight" activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5448,7 +5451,7 @@
       </c>
       <c r="H126" s="35"/>
       <c r="I126" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5469,7 +5472,7 @@
       </c>
       <c r="H127" s="35"/>
       <c r="I127" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -5490,7 +5493,7 @@
       </c>
       <c r="H128" s="35"/>
       <c r="I128" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
@@ -5511,7 +5514,7 @@
       </c>
       <c r="H129" s="35"/>
       <c r="I129" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5530,7 +5533,7 @@
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -5551,7 +5554,7 @@
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -5572,7 +5575,7 @@
       </c>
       <c r="H132" s="3"/>
       <c r="I132" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -5593,7 +5596,7 @@
       </c>
       <c r="H133" s="35"/>
       <c r="I133" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -5614,7 +5617,7 @@
       </c>
       <c r="H134" s="35"/>
       <c r="I134" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5625,7 +5628,7 @@
         <v>85</v>
       </c>
       <c r="C135" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D135" s="35"/>
       <c r="E135" s="35"/>
@@ -5635,7 +5638,7 @@
       </c>
       <c r="H135" s="35"/>
       <c r="I135" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
@@ -5656,7 +5659,7 @@
       </c>
       <c r="H136" s="35"/>
       <c r="I136" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -5675,7 +5678,7 @@
       </c>
       <c r="H137" s="3"/>
       <c r="I137" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5683,7 +5686,7 @@
         <v>222</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>197</v>
+        <v>248</v>
       </c>
       <c r="C138" s="3">
         <v>8</v>
@@ -5696,7 +5699,7 @@
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="20" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
doc's, Persistencia Final Update, Altera??o ficheiro build.bat
</commit_message>
<xml_diff>
--- a/docs/Log_Gestao_Projecto_aluno1_1100554.xlsx
+++ b/docs/Log_Gestao_Projecto_aluno1_1100554.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="7935" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação" sheetId="3" r:id="rId1"/>
@@ -1537,9 +1537,6 @@
     <t>Exportar/Importar dados de base de dados (Hibernate)</t>
   </si>
   <si>
-    <t>Desenvolvimento codigo importação/Exportaca</t>
-  </si>
-  <si>
     <t>Desenvolver aspecto gráfico folha de cálculo em HTML</t>
   </si>
   <si>
@@ -1661,6 +1658,9 @@
   </si>
   <si>
     <t>21.5</t>
+  </si>
+  <si>
+    <t>Desenvolvimento codigo importação/Exportação</t>
   </si>
 </sst>
 </file>
@@ -2952,11 +2952,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="9" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3489,13 +3489,13 @@
         <v>20</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C29" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="D29" s="32" t="s">
         <v>332</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>333</v>
       </c>
       <c r="E29" s="3">
         <v>6</v>
@@ -3512,13 +3512,13 @@
         <v>21</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C30" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="D30" s="32" t="s">
         <v>334</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>335</v>
       </c>
       <c r="E30" s="3">
         <v>7</v>
@@ -3602,11 +3602,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="C91" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="11" topLeftCell="C192" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="K184" sqref="K184"/>
+      <selection pane="bottomRight" activeCell="J204" sqref="J204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6978,7 +6978,7 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>79</v>
@@ -6994,12 +6994,12 @@
       </c>
       <c r="H195" s="35"/>
       <c r="I195" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>80</v>
@@ -7015,12 +7015,12 @@
       </c>
       <c r="H196" s="35"/>
       <c r="I196" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B197" s="32" t="s">
         <v>81</v>
@@ -7036,12 +7036,12 @@
       </c>
       <c r="H197" s="35"/>
       <c r="I197" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B198" s="32" t="s">
         <v>303</v>
@@ -7055,15 +7055,15 @@
       </c>
       <c r="H198" s="3"/>
       <c r="I198" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>304</v>
+        <v>311</v>
+      </c>
+      <c r="B199" s="32" t="s">
+        <v>345</v>
       </c>
       <c r="C199" s="3">
         <v>5</v>
@@ -7076,12 +7076,12 @@
       </c>
       <c r="H199" s="3"/>
       <c r="I199" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>79</v>
@@ -7097,12 +7097,12 @@
       </c>
       <c r="H200" s="3"/>
       <c r="I200" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>80</v>
@@ -7118,12 +7118,12 @@
       </c>
       <c r="H201" s="3"/>
       <c r="I201" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="202" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B202" s="32" t="s">
         <v>81</v>
@@ -7139,12 +7139,12 @@
       </c>
       <c r="H202" s="3"/>
       <c r="I202" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B203" s="32" t="s">
         <v>301</v>
@@ -7158,15 +7158,15 @@
       </c>
       <c r="H203" s="3"/>
       <c r="I203" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C204" s="3">
         <v>8</v>
@@ -7179,15 +7179,15 @@
       </c>
       <c r="H204" s="3"/>
       <c r="I204" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="205" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B205" s="56" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C205" s="3">
         <v>8</v>
@@ -7200,15 +7200,15 @@
       </c>
       <c r="H205" s="3"/>
       <c r="I205" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C206" s="3">
         <v>8</v>
@@ -7221,15 +7221,15 @@
       </c>
       <c r="H206" s="3"/>
       <c r="I206" s="20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B207" s="32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C207" s="3">
         <v>2</v>
@@ -7247,10 +7247,10 @@
     </row>
     <row r="208" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B208" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C208" s="3">
         <v>3</v>
@@ -7268,10 +7268,10 @@
     </row>
     <row r="209" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B209" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C209" s="3">
         <v>4</v>
@@ -7289,10 +7289,10 @@
     </row>
     <row r="210" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B210" s="32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C210" s="3">
         <v>5</v>
@@ -7310,10 +7310,10 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B211" s="32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C211" s="3">
         <v>7</v>
@@ -7331,10 +7331,10 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B212" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C212" s="3">
         <v>7</v>
@@ -7352,10 +7352,10 @@
     </row>
     <row r="213" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B213" s="32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C213" s="3">
         <v>6</v>
@@ -7373,10 +7373,10 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B214" s="32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C214" s="3">
         <v>5</v>
@@ -7394,10 +7394,10 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B215" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C215" s="3">
         <v>2</v>
@@ -7415,10 +7415,10 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B216" s="32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C216" s="3">
         <v>2</v>

</xml_diff>